<commit_message>
Closes #3. Fixed SSRs names in cvs file and updates examples
</commit_message>
<xml_diff>
--- a/shiny-server/www/SSR-ID/www/SSR_Example_Data_ramorum.xlsx
+++ b/shiny-server/www/SSR-ID/www/SSR_Example_Data_ramorum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tabimaj/Documents/microbe-ID/shiny-server/www/SSR-ID/www/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="17040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="reduced_database.txt.csv" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name	Lineage	PrMS6	PrMS9c3	ILVOPrMS132/PrMS39a	PRMS45	PrMS43a	PrMS43b	ILVOPrMS133/PrMS43a	KI18	KI64	KI82ab	KI82a	KI82b	ILVOPrMS79ab	ILVOPrMS131	ILVOPrMS145abc	PrMS145a	PrMS145b	PrMS145c</t>
   </si>
@@ -106,88 +111,55 @@
     <t>ILVOPrMS131</t>
   </si>
   <si>
-    <t>sample1</t>
-  </si>
-  <si>
-    <t>sample2</t>
-  </si>
-  <si>
-    <t>169/172</t>
-  </si>
-  <si>
-    <t>221/231</t>
-  </si>
-  <si>
-    <t>136/252</t>
-  </si>
-  <si>
-    <t>172/192</t>
-  </si>
-  <si>
-    <t>373/489</t>
-  </si>
-  <si>
-    <t>224/278</t>
-  </si>
-  <si>
-    <t>347/383</t>
-  </si>
-  <si>
     <t>150/234</t>
   </si>
   <si>
     <t>221/221</t>
   </si>
   <si>
-    <t>152/158</t>
-  </si>
-  <si>
-    <t>173/173</t>
-  </si>
-  <si>
-    <t>226/226</t>
-  </si>
-  <si>
-    <t>349/365</t>
-  </si>
-  <si>
-    <t>278/342</t>
-  </si>
-  <si>
-    <t>169/169</t>
-  </si>
-  <si>
-    <t>223/229</t>
-  </si>
-  <si>
-    <t>142/148</t>
-  </si>
-  <si>
-    <t>168/192</t>
-  </si>
-  <si>
-    <t>149/149</t>
-  </si>
-  <si>
-    <t>222/266</t>
-  </si>
-  <si>
-    <t>355/405</t>
-  </si>
-  <si>
-    <t>394/406</t>
-  </si>
-  <si>
-    <t>0/0</t>
-  </si>
-  <si>
     <t>ILVOPrMS133/PrMS43ab</t>
   </si>
   <si>
-    <t>sample3</t>
-  </si>
-  <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>NA1_sample1</t>
+  </si>
+  <si>
+    <t>NA2_sample2</t>
+  </si>
+  <si>
+    <t>165/168</t>
+  </si>
+  <si>
+    <t>216/226</t>
+  </si>
+  <si>
+    <t>372/489</t>
+  </si>
+  <si>
+    <t>130/246</t>
+  </si>
+  <si>
+    <t>219/275</t>
+  </si>
+  <si>
+    <t>342/379</t>
+  </si>
+  <si>
+    <t>216/216</t>
+  </si>
+  <si>
+    <t>161/174</t>
+  </si>
+  <si>
+    <t>145/151</t>
+  </si>
+  <si>
+    <t>344/360</t>
+  </si>
+  <si>
+    <t>274/342</t>
   </si>
 </sst>
 </file>
@@ -310,6 +282,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -639,99 +616,99 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -739,11 +716,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -752,16 +724,16 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -781,7 +753,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>25</v>
@@ -793,109 +765,84 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>51</v>
-      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>